<commit_message>
Updates to Unit Conversion
</commit_message>
<xml_diff>
--- a/kb/unit-converter/Pressure.xlsx
+++ b/kb/unit-converter/Pressure.xlsx
@@ -1,21 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmcclure\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pumpsorg.sharepoint.com/sites/EngineeringDataLibrary/Shared Documents/General/Work Group(s)/Unit Conversions/unit-converter/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="88" documentId="11_692AFBE2A705FB02C94EBC595144036B5F37C29D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E12884C2-2BF6-4ADB-95A2-8E2F841482E8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="500"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -24,11 +39,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Measure Label</t>
   </si>
   <si>
+    <t>Pressure</t>
+  </si>
+  <si>
     <t>Cell B2 Must be the name of the measure</t>
   </si>
   <si>
@@ -41,6 +59,9 @@
     <t>Image</t>
   </si>
   <si>
+    <t>Pressure.png</t>
+  </si>
+  <si>
     <t>Icon, must be populated.  The png should be in the images directory of the edb source folder</t>
   </si>
   <si>
@@ -51,6 +72,9 @@
   </si>
   <si>
     <t>Factor</t>
+  </si>
+  <si>
+    <t>atm</t>
   </si>
   <si>
     <r>
@@ -83,44 +107,74 @@
     </r>
   </si>
   <si>
+    <t>bar</t>
+  </si>
+  <si>
     <t>For all other units, the factor should be the DIVISOR, in order to get from the unit on this row, to the standard unit in row 6.  For example, if you have 5000mm, then dividing by 1000 gets you 5 meters.</t>
   </si>
   <si>
+    <t>ftH2O 39.2&amp;degF (4&amp;degC)</t>
+  </si>
+  <si>
     <t>You can place as many units as you want – the system will read until there is an empty cell in column A</t>
   </si>
   <si>
-    <t>Pressure</t>
-  </si>
-  <si>
-    <t>atmospheres</t>
-  </si>
-  <si>
-    <t>bar</t>
-  </si>
-  <si>
-    <t>kilopascal</t>
-  </si>
-  <si>
-    <t>kilopounds per square inch</t>
-  </si>
-  <si>
-    <t>megapascal</t>
-  </si>
-  <si>
-    <t>pascal</t>
-  </si>
-  <si>
-    <t>pounds per square inch</t>
-  </si>
-  <si>
-    <t>Pressure.png</t>
+    <t>ftH2O 68&amp;degF (20&amp;degC)</t>
+  </si>
+  <si>
+    <t>inHg 32&amp;degF (0&amp;degC)</t>
+  </si>
+  <si>
+    <t>kg/cm&amp;sup2</t>
+  </si>
+  <si>
+    <t>kg/m&amp;sup2</t>
+  </si>
+  <si>
+    <t>Divided by</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>kg/mm&amp;sup2</t>
+  </si>
+  <si>
+    <t>kN/m&amp;sup2</t>
+  </si>
+  <si>
+    <t>SG to 39.2F 4C</t>
+  </si>
+  <si>
+    <t>kPa</t>
+  </si>
+  <si>
+    <t>to kPa</t>
+  </si>
+  <si>
+    <t>ksi</t>
+  </si>
+  <si>
+    <t>mmHg 32&amp;degF (0&amp;degC)</t>
+  </si>
+  <si>
+    <t>MPa</t>
+  </si>
+  <si>
+    <t>N/m&amp;sup2</t>
+  </si>
+  <si>
+    <t>Pa</t>
+  </si>
+  <si>
+    <t>psi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -170,7 +224,7 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -182,10 +236,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,137 +589,236 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="46.42578125" customWidth="1"/>
     <col min="4" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.899999999999999">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="54.75" customHeight="1">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="52.9">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1">
         <v>1.01325</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="24">
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
+        <v>33.899524252420555</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="12.75">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>33.959632854853496</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" ht="12.75">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>29.921331923765202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="12.75">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>1.0332274527998857</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="12.75">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>10332.274527998859</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="12.75">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>1.0332274527998859E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="12.75">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14">
         <v>101.325</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1">
+      <c r="C14">
+        <v>1.0017731400000001</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="12.75">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1">
+        <v>101.325</v>
+      </c>
+      <c r="C15">
+        <v>2.9889800000000002</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="12.75">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="1">
         <v>1.46959E-2</v>
       </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="6">
+      <c r="C16">
+        <v>3.3863799999999999</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="12.75">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17">
+        <v>760.00183086363609</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="12.75">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18">
         <v>0.101325</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11">
+    <row r="19" spans="1:2" ht="12.75">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19">
         <v>101325</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12">
+    <row r="20" spans="1:2" ht="12.75">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20">
+        <v>101325</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="12.75">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21">
         <v>14.6959</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:B21">
+    <sortCondition ref="A7:A21"/>
+  </sortState>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -671,4 +826,273 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C5F168F66F91CF43BAEE65DC9E9CF3DF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="012c7fef03233136f3b92728f80e18f9">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8da57d07-bd53-4918-9441-156ccef8128a" xmlns:ns3="32f445ef-0db1-4ff5-a403-59aa008b5549" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8bc58cbf5cc050e49b481be3a36a2ee3" ns2:_="" ns3:_="">
+    <xsd:import namespace="8da57d07-bd53-4918-9441-156ccef8128a"/>
+    <xsd:import namespace="32f445ef-0db1-4ff5-a403-59aa008b5549"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="8da57d07-bd53-4918-9441-156ccef8128a" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="18c22185-266d-4dbf-8bc9-f312ea01a8ea" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="19" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="22" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="32f445ef-0db1-4ff5-a403-59aa008b5549" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{72fdf2aa-35ea-45bb-903c-e2487b42d74a}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="32f445ef-0db1-4ff5-a403-59aa008b5549">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithUsers" ma:index="20" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="21" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8da57d07-bd53-4918-9441-156ccef8128a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="32f445ef-0db1-4ff5-a403-59aa008b5549" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94F0B47C-5758-4FDE-BB4D-5106869A8C6B}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA9030FD-2A85-4190-8029-A2F0D4C78DA7}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9FC9AC8-0A48-4F79-8D4D-FF7F52E168DF}"/>
 </file>
</xml_diff>

<commit_message>
12-5-23 late updates with Pete
</commit_message>
<xml_diff>
--- a/kb/unit-converter/Pressure.xlsx
+++ b/kb/unit-converter/Pressure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pumpsorg.sharepoint.com/sites/EngineeringDataLibrary/Shared Documents/General/Work Group(s)/Unit Conversions/unit-converter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="11_692AFBE2A705FB02C94EBC595144036B5F37C29D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E12884C2-2BF6-4ADB-95A2-8E2F841482E8}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="11_692AFBE2A705FB02C94EBC595144036B5F37C29D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D263FFF-CE6D-457B-9EEB-B94E64268E40}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Measure Label</t>
   </si>
@@ -113,61 +113,67 @@
     <t>For all other units, the factor should be the DIVISOR, in order to get from the unit on this row, to the standard unit in row 6.  For example, if you have 5000mm, then dividing by 1000 gets you 5 meters.</t>
   </si>
   <si>
+    <t>psi</t>
+  </si>
+  <si>
+    <t>You can place as many units as you want – the system will read until there is an empty cell in column A</t>
+  </si>
+  <si>
+    <t>ksi</t>
+  </si>
+  <si>
+    <t>Pa</t>
+  </si>
+  <si>
+    <t>kPa</t>
+  </si>
+  <si>
+    <t>MPa</t>
+  </si>
+  <si>
     <t>ftH2O 39.2&amp;degF (4&amp;degC)</t>
   </si>
   <si>
-    <t>You can place as many units as you want – the system will read until there is an empty cell in column A</t>
-  </si>
-  <si>
     <t>ftH2O 68&amp;degF (20&amp;degC)</t>
   </si>
   <si>
+    <t>Divided by</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>mH2O 39.2&amp;degF (4&amp;degC)</t>
+  </si>
+  <si>
+    <t>mH2O 68&amp;degF (20&amp;degC)</t>
+  </si>
+  <si>
+    <t>SG to 39.2F 4C</t>
+  </si>
+  <si>
     <t>inHg 32&amp;degF (0&amp;degC)</t>
   </si>
   <si>
+    <t>to kPa</t>
+  </si>
+  <si>
+    <t>mmHg 32&amp;degF (0&amp;degC)</t>
+  </si>
+  <si>
     <t>kg/cm&amp;sup2</t>
   </si>
   <si>
     <t>kg/m&amp;sup2</t>
   </si>
   <si>
-    <t>Divided by</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>kg/mm&amp;sup2</t>
   </si>
   <si>
     <t>kN/m&amp;sup2</t>
   </si>
   <si>
-    <t>SG to 39.2F 4C</t>
-  </si>
-  <si>
-    <t>kPa</t>
-  </si>
-  <si>
-    <t>to kPa</t>
-  </si>
-  <si>
-    <t>ksi</t>
-  </si>
-  <si>
-    <t>mmHg 32&amp;degF (0&amp;degC)</t>
-  </si>
-  <si>
-    <t>MPa</t>
-  </si>
-  <si>
     <t>N/m&amp;sup2</t>
-  </si>
-  <si>
-    <t>Pa</t>
-  </si>
-  <si>
-    <t>psi</t>
   </si>
 </sst>
 </file>
@@ -590,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15"/>
@@ -680,7 +686,7 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>33.899524252420555</v>
+        <v>14.6959</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>16</v>
@@ -690,8 +696,8 @@
       <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9">
-        <v>33.959632854853496</v>
+      <c r="B9" s="1">
+        <v>1.46959E-2</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -700,124 +706,172 @@
         <v>18</v>
       </c>
       <c r="B10">
-        <v>29.921331923765202</v>
-      </c>
+        <v>101325</v>
+      </c>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:4" ht="12.75">
       <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B11">
-        <v>1.0332274527998857</v>
-      </c>
+      <c r="B11" s="1">
+        <v>101.325</v>
+      </c>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:4" ht="12.75">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12">
-        <v>10332.274527998859</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" t="s">
-        <v>22</v>
+        <v>0.101325</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12.75">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13">
-        <v>1.0332274527998859E-2</v>
+        <v>33.899524252420555</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75">
       <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>33.959632854853496</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
         <v>24</v>
-      </c>
-      <c r="B14">
-        <v>101.325</v>
-      </c>
-      <c r="C14">
-        <v>1.0017731400000001</v>
-      </c>
-      <c r="D14" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75">
       <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="1">
-        <v>101.325</v>
-      </c>
-      <c r="C15">
-        <v>2.9889800000000002</v>
-      </c>
-      <c r="D15" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>10.332595330843233</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75">
       <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1.46959E-2</v>
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <v>10.350916468928165</v>
       </c>
       <c r="C16">
-        <v>3.3863799999999999</v>
+        <v>1.0017731400000001</v>
       </c>
       <c r="D16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="12.75">
+    <row r="17" spans="1:4" ht="12.75">
       <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <v>29.921331923765202</v>
+      </c>
+      <c r="C17">
+        <v>2.9889800000000002</v>
+      </c>
+      <c r="D17" t="s">
         <v>29</v>
       </c>
-      <c r="B17">
-        <v>760.00183086363609</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="12.75">
+    </row>
+    <row r="18" spans="1:4" ht="12.75">
       <c r="A18" t="s">
         <v>30</v>
       </c>
       <c r="B18">
-        <v>0.101325</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="12.75">
+        <v>760.00183086363609</v>
+      </c>
+      <c r="C18">
+        <v>3.3863799999999999</v>
+      </c>
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="12.75">
       <c r="A19" t="s">
         <v>31</v>
       </c>
       <c r="B19">
-        <v>101325</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="12.75">
+        <v>1.0332274527998857</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="12.75">
       <c r="A20" t="s">
         <v>32</v>
       </c>
       <c r="B20">
-        <v>101325</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="12.75">
+        <v>10332.274527998859</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="12.75">
       <c r="A21" t="s">
         <v>33</v>
       </c>
       <c r="B21">
-        <v>14.6959</v>
-      </c>
-    </row>
+        <v>1.0332274527998859E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="12.75">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22">
+        <v>101.325</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="12.75">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23">
+        <v>101325</v>
+      </c>
+      <c r="C23">
+        <f>B8/B17</f>
+        <v>0.4911512641697508</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="12.75">
+      <c r="C24">
+        <f>B17/B13</f>
+        <v>0.88264754693802838</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="12.75">
+      <c r="C25">
+        <f>B11/B18</f>
+        <v>0.13332204724409449</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="12.75">
+      <c r="C26">
+        <f>B11/B16</f>
+        <v>9.7889882798457339</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="12.75">
+      <c r="C27">
+        <f>B15/B11</f>
+        <v>0.10197478737570424</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="12.75"/>
+    <row r="29" spans="1:4" ht="12.75"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:B21">
-    <sortCondition ref="A7:A21"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:B24">
+    <sortCondition ref="A7:A24"/>
   </sortState>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -829,15 +883,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C5F168F66F91CF43BAEE65DC9E9CF3DF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="012c7fef03233136f3b92728f80e18f9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8da57d07-bd53-4918-9441-156ccef8128a" xmlns:ns3="32f445ef-0db1-4ff5-a403-59aa008b5549" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8bc58cbf5cc050e49b481be3a36a2ee3" ns2:_="" ns3:_="">
     <xsd:import namespace="8da57d07-bd53-4918-9441-156ccef8128a"/>
@@ -1074,7 +1119,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="8da57d07-bd53-4918-9441-156ccef8128a">
@@ -1085,14 +1130,23 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94F0B47C-5758-4FDE-BB4D-5106869A8C6B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA9030FD-2A85-4190-8029-A2F0D4C78DA7}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA9030FD-2A85-4190-8029-A2F0D4C78DA7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9FC9AC8-0A48-4F79-8D4D-FF7F52E168DF}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9FC9AC8-0A48-4F79-8D4D-FF7F52E168DF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94F0B47C-5758-4FDE-BB4D-5106869A8C6B}"/>
 </file>
</xml_diff>

<commit_message>
Teamknight 07 13 24 (#98)
* EDL-26

* EDL-30, 31, 33

* EDL-34, 35, 36, 37

* EDL-35

* Typo EDL-31

* EDL-40,

* EDL-41

* EDL-42

* EDL-41

* EDL 43 (part),  44

* Fix EDL-36

* EDL-39 partial

* Updated EDL-40

* EDL-29

* EDL-47

* EDL-48

* EDL-46

* menu work

* EDL-46

* EDL-46 continued

* EDL-46 - clean out MathJax.  Couldn't find where it was used anywhere.

* Fix MathJax

* EDL-46, also adjust table sizes if needed for definitions, etc.

* fix padding

* fix padding for icon

* minor mods

* EDL-39 Flanges

* EDL-49 ReBranding

* EDL-49 updates

* minor fixes

* typo

* Fix equation

* upsell links

* fix tank calculators

* EDL-43 Update Atmospheric Calculator

* Fix Section IV tables that included STANDARD Column

* Fix datatables

* Update About title

* No collapse and search fix

* scroll first search into view
</commit_message>
<xml_diff>
--- a/kb/unit-converter/Pressure.xlsx
+++ b/kb/unit-converter/Pressure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pumpsorg.sharepoint.com/sites/EngineeringDataLibrary/Shared Documents/General/Work Group(s)/Unit Conversions/unit-converter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\edb\kb\unit-converter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="11_692AFBE2A705FB02C94EBC595144036B5F37C29D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D263FFF-CE6D-457B-9EEB-B94E64268E40}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18E319A-C03C-4E7E-B36B-F41B7B90BEB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2700" yWindow="1800" windowWidth="19410" windowHeight="13575" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,15 +31,12 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
   <si>
     <t>Measure Label</t>
   </si>
@@ -175,17 +172,84 @@
   <si>
     <t>N/m&amp;sup2</t>
   </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>standard atmosphere</t>
+  </si>
+  <si>
+    <t>pound per square inch</t>
+  </si>
+  <si>
+    <t>kilopound per square inch</t>
+  </si>
+  <si>
+    <t>pascal</t>
+  </si>
+  <si>
+    <t>kilopascal</t>
+  </si>
+  <si>
+    <t>megapascal</t>
+  </si>
+  <si>
+    <t>foot of water at 39.2°F or 4°C</t>
+  </si>
+  <si>
+    <t>foot of water at 68°F or 20°C</t>
+  </si>
+  <si>
+    <t>meter of water at 39.2°F or 4°C</t>
+  </si>
+  <si>
+    <t>meter of water at 68°F or 20°C</t>
+  </si>
+  <si>
+    <t>inch of mercury at 32°F or 0°C</t>
+  </si>
+  <si>
+    <t>millimeter of mercury at 32°F or 0°C</t>
+  </si>
+  <si>
+    <t>kilogram per square centimeter</t>
+  </si>
+  <si>
+    <t>kilogram per square meter</t>
+  </si>
+  <si>
+    <t>kilogram per square millimeter</t>
+  </si>
+  <si>
+    <t>kilonewton per square meter</t>
+  </si>
+  <si>
+    <t>newton per square meter</t>
+  </si>
+  <si>
+    <t>Default From Row</t>
+  </si>
+  <si>
+    <t>Default To Row</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -225,21 +289,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -248,9 +313,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{E03FD64E-F459-4A9A-B023-061387C0CCE7}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -596,282 +663,361 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.15"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.140625" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="46.42578125" customWidth="1"/>
-    <col min="4" max="1025" width="11.5703125"/>
+    <col min="2" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="46.42578125" customWidth="1"/>
+    <col min="5" max="1026" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.899999999999999">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="1">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="4" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" ht="54.75" customHeight="1">
-      <c r="A6" t="s">
+      <c r="C7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="52.9">
-      <c r="A7" t="s">
+    <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B9" s="1">
         <v>1.01325</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="24">
-      <c r="A8" t="s">
+    <row r="10" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B8">
+      <c r="B10">
         <v>14.6959</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="12.75">
-      <c r="A9" t="s">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B11" s="1">
         <v>1.46959E-2</v>
       </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" ht="12.75">
-      <c r="A10" t="s">
+      <c r="C11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="B10">
+      <c r="B12">
         <v>101325</v>
       </c>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" ht="12.75">
-      <c r="A11" t="s">
+      <c r="C12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B13" s="1">
         <v>101.325</v>
       </c>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" ht="12.75">
-      <c r="A12" t="s">
+      <c r="C13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B12">
+      <c r="B14">
         <v>0.101325</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="12.75">
-      <c r="A13" t="s">
+      <c r="C14" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="B13">
+      <c r="B15">
         <v>33.899524252420555</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="12.75">
-      <c r="A14" t="s">
+      <c r="C15" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="B14">
+      <c r="B16">
         <v>33.959632854853496</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="12.75">
-      <c r="A15" t="s">
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>25</v>
       </c>
-      <c r="B15">
+      <c r="B17">
         <v>10.332595330843233</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="12.75">
-      <c r="A16" t="s">
+      <c r="C17" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B16">
+      <c r="B18">
         <v>10.350916468928165</v>
       </c>
-      <c r="C16">
+      <c r="C18" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18">
         <v>1.0017731400000001</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="12.75">
-      <c r="A17" t="s">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>28</v>
       </c>
-      <c r="B17">
+      <c r="B19">
         <v>29.921331923765202</v>
       </c>
-      <c r="C17">
+      <c r="C19" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19">
         <v>2.9889800000000002</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="12.75">
-      <c r="A18" t="s">
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>30</v>
       </c>
-      <c r="B18">
+      <c r="B20">
         <v>760.00183086363609</v>
       </c>
-      <c r="C18">
+      <c r="C20" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20">
         <v>3.3863799999999999</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="12.75">
-      <c r="A19" t="s">
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>31</v>
       </c>
-      <c r="B19">
+      <c r="B21">
         <v>1.0332274527998857</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="12.75">
-      <c r="A20" t="s">
+      <c r="C21" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>32</v>
       </c>
-      <c r="B20">
+      <c r="B22">
         <v>10332.274527998859</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="12.75">
-      <c r="A21" t="s">
+      <c r="C22" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>33</v>
       </c>
-      <c r="B21">
+      <c r="B23">
         <v>1.0332274527998859E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="12.75">
-      <c r="A22" t="s">
+      <c r="C23" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>34</v>
       </c>
-      <c r="B22">
+      <c r="B24">
         <v>101.325</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="12.75">
-      <c r="A23" t="s">
+      <c r="C24" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>35</v>
       </c>
-      <c r="B23">
+      <c r="B25">
         <v>101325</v>
       </c>
-      <c r="C23">
-        <f>B8/B17</f>
+      <c r="C25" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25">
+        <f>B10/B19</f>
         <v>0.4911512641697508</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="12.75">
-      <c r="C24">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <f>B19/B15</f>
+        <v>0.88264754693802838</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <f>B13/B20</f>
+        <v>0.13332204724409449</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <f>B13/B18</f>
+        <v>9.7889882798457339</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D29">
         <f>B17/B13</f>
-        <v>0.88264754693802838</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="12.75">
-      <c r="C25">
-        <f>B11/B18</f>
-        <v>0.13332204724409449</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="12.75">
-      <c r="C26">
-        <f>B11/B16</f>
-        <v>9.7889882798457339</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="12.75">
-      <c r="C27">
-        <f>B15/B11</f>
         <v>0.10197478737570424</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="12.75"/>
-    <row r="29" spans="1:4" ht="12.75"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:B24">
-    <sortCondition ref="A7:A24"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:B26">
+    <sortCondition ref="A9:A26"/>
   </sortState>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -883,6 +1029,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C5F168F66F91CF43BAEE65DC9E9CF3DF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="012c7fef03233136f3b92728f80e18f9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8da57d07-bd53-4918-9441-156ccef8128a" xmlns:ns3="32f445ef-0db1-4ff5-a403-59aa008b5549" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8bc58cbf5cc050e49b481be3a36a2ee3" ns2:_="" ns3:_="">
     <xsd:import namespace="8da57d07-bd53-4918-9441-156ccef8128a"/>
@@ -1119,7 +1274,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="8da57d07-bd53-4918-9441-156ccef8128a">
@@ -1130,23 +1285,40 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA9030FD-2A85-4190-8029-A2F0D4C78DA7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94F0B47C-5758-4FDE-BB4D-5106869A8C6B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9FC9AC8-0A48-4F79-8D4D-FF7F52E168DF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA9030FD-2A85-4190-8029-A2F0D4C78DA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8da57d07-bd53-4918-9441-156ccef8128a"/>
+    <ds:schemaRef ds:uri="32f445ef-0db1-4ff5-a403-59aa008b5549"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94F0B47C-5758-4FDE-BB4D-5106869A8C6B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9FC9AC8-0A48-4F79-8D4D-FF7F52E168DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8da57d07-bd53-4918-9441-156ccef8128a"/>
+    <ds:schemaRef ds:uri="32f445ef-0db1-4ff5-a403-59aa008b5549"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>